<commit_message>
LOMT-1839 report changes + functions adjusted
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
     <sheet name="Alignment Type" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alignment Type'!$A$1:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alignment Type'!$A$1:$C$21</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t xml:space="preserve">Product </t>
   </si>
@@ -157,9 +157,6 @@
 </t>
   </si>
   <si>
-    <t>2/3</t>
-  </si>
-  <si>
     <t>Intermediary 6
 Intermediary 7</t>
   </si>
@@ -171,6 +168,13 @@
   </si>
   <si>
     <t>0/0</t>
+  </si>
+  <si>
+    <t>2/4</t>
+  </si>
+  <si>
+    <t>Intermediary 12
+Intermediary 8</t>
   </si>
 </sst>
 </file>
@@ -556,7 +560,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,13 +672,13 @@
         <v>39</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
+      <c r="J7" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -694,7 +698,7 @@
         <v>40</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -711,7 +715,7 @@
         <v>40</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -808,10 +812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -963,47 +967,47 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="B15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="11" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="B17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1011,36 +1015,47 @@
         <v>5</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="16" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="15" t="s">
+      <c r="B20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C20"/>
+  <autoFilter ref="A1:C21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
partial commit - gap analysis
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lomt_automation\src\main\java\lomt\pearson\fileupload\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Alignment Type" sheetId="2" r:id="rId2"/>
+    <sheet name="GapAnalysis" sheetId="3" r:id="rId2"/>
+    <sheet name="Alignment Type" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alignment Type'!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alignment Type'!$A$1:$C$21</definedName>
   </definedNames>
-  <calcPr calcId="125725" refMode="R1C1"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
   <si>
     <t xml:space="preserve">Product </t>
   </si>
@@ -176,12 +182,84 @@
     <t>Intermediary 12
 Intermediary 8</t>
   </si>
+  <si>
+    <t>Automation Report Test-2</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Automation Report Test (US Grade K-12)</t>
+  </si>
+  <si>
+    <t>TEST 1 (US Grade K-12)</t>
+  </si>
+  <si>
+    <t>Child-Mapping</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Add Note(Comments)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gap Analysis </t>
+  </si>
+  <si>
+    <t>Text Types and Purposes - LEVEL 2.</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>TEST 2 (US Grade K-12)</t>
+  </si>
+  <si>
+    <t>Related</t>
+  </si>
+  <si>
+    <t>Write arguments to support claims in an analysis of substantive topics or texts, using valid reasoning and relevant and sufficient evidence - LEVEL 3.</t>
+  </si>
+  <si>
+    <t>TEST 3 (US Grade K-12)</t>
+  </si>
+  <si>
+    <t>Broad</t>
+  </si>
+  <si>
+    <t>Reading LEVEL 4.</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>TEST 4 (US Grade K-12)</t>
+  </si>
+  <si>
+    <t>Reading LOWEST LEVEL</t>
+  </si>
+  <si>
+    <t>Conventions of Standard English (US Grade K-12)</t>
+  </si>
+  <si>
+    <t>Narrow</t>
+  </si>
+  <si>
+    <t>Lowest node alignment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +364,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,21 +641,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
@@ -585,7 +666,7 @@
     <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -632,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60">
+    <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -658,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -684,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -704,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -721,7 +802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -729,79 +810,79 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
   </sheetData>
@@ -811,19 +892,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="37.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -834,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -845,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
@@ -856,7 +1055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -867,7 +1066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -878,7 +1077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -889,7 +1088,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -900,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>24</v>
       </c>
@@ -911,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -922,7 +1121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -933,7 +1132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
@@ -944,7 +1143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>3</v>
       </c>
@@ -955,7 +1154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
@@ -966,7 +1165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
@@ -977,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>24</v>
       </c>
@@ -988,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -999,7 +1198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1209,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
@@ -1043,7 +1242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
LOMT-1840 - code commit
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
@@ -429,7 +429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -464,7 +464,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -896,7 +896,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
code commit of LOMT-1838
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lomt_automation\src\main\java\lomt\pearson\fileupload\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="505" activeTab="1"/>
   </bookViews>
@@ -15,8 +20,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alignment Type'!$A$1:$C$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -253,8 +258,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,7 +429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -459,7 +464,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -636,21 +641,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
@@ -661,7 +666,7 @@
     <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -684,7 +689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -708,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60">
+    <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -734,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30">
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -760,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -780,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -797,7 +802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -805,79 +810,79 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
   </sheetData>
@@ -887,14 +892,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -904,7 +909,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
@@ -912,7 +917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>50</v>
       </c>
@@ -932,7 +937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -952,7 +957,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
@@ -963,7 +968,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
@@ -974,7 +979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>66</v>
       </c>
@@ -985,7 +990,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>69</v>
       </c>
@@ -1005,19 +1010,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -1028,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
@@ -1050,7 +1055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1072,7 +1077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1083,7 +1088,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1094,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>24</v>
       </c>
@@ -1105,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1116,7 +1121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1127,7 +1132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
@@ -1138,7 +1143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>3</v>
       </c>
@@ -1149,7 +1154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
@@ -1160,7 +1165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
@@ -1171,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1193,7 +1198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
@@ -1204,7 +1209,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
@@ -1215,7 +1220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
@@ -1237,7 +1242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Reports restructuring of code
</commit_message>
<xml_diff>
--- a/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
+++ b/src/main/java/lomt/pearson/fileupload/reports/Report_Automation_Align_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Alignment Type" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alignment Type'!$A$1:$C$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alignment Type'!$A$4:$C$24</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="74">
   <si>
     <t xml:space="preserve">Product </t>
   </si>
@@ -253,6 +253,65 @@
   </si>
   <si>
     <t>Lowest node alignment</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Product : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Product_TOC_Report_Ingestion.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Intermediary : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intermediary_Report_Ingestion.xlsx</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Curriculum Standard : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Curriculum_Report_IngestionTemplate_small-Target.xml</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -320,7 +379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -328,11 +387,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -342,33 +416,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +736,7 @@
   <dimension ref="B4:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,30 +994,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1011,250 +1095,272 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="B6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B8" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B9" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="B11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="B18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B20" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B21" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C21" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C22" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C23" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" s="15" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C21"/>
+  <autoFilter ref="A4:C24"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>